<commit_message>
Aanpassingen n.a.v. testresultaten dd. 12-10-2022
</commit_message>
<xml_diff>
--- a/Overgangsrecht+TAM/Testresultaat_additional-validator-rules-2012v0.08-b-RC.sch-2008v1.18-b-RC.sch_TAM-uitgebreid.xlsx
+++ b/Overgangsrecht+TAM/Testresultaat_additional-validator-rules-2012v0.08-b-RC.sch-2008v1.18-b-RC.sch_TAM-uitgebreid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gijsk\Documents\GitHub\imro-dev\Overgangsrecht+TAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3699387D-8D1A-46E2-9E58-47359A235AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAF5927-3F89-4C63-98AE-E067DA512B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B9409DF-38CF-4439-A4D2-12BFE7E549DF}"/>
   </bookViews>
@@ -286,98 +286,124 @@
     <t>1b_IOW_toestaan_planstatus_geconsolideerd</t>
   </si>
   <si>
-    <t>Testresultaat
+    <t>1c_datum_na_IOW_ontwerp_TAMuitgebreid</t>
+  </si>
+  <si>
+    <t>1e: datum na_IOW_ontwerp_TAMuitgebreid  NL.IMRO.0000.EZKip18GaswTern-2001</t>
+  </si>
+  <si>
+    <t>1c_datum_na_IOW TAM_uitgebreid</t>
+  </si>
+  <si>
+    <t>1c_datum_na_IOW TAM_uitgebreid - NL.IMRO.9923.phVerordening006B-va01</t>
+  </si>
+  <si>
+    <t>1c_datum_na_IOW_TAM_uitgebreid</t>
+  </si>
+  <si>
+    <t>1c_datum_na_IOW_TAM_uitgebreid - NL.IMRO.9926.RA0318SLAPPEDEL8A-VA01</t>
+  </si>
+  <si>
+    <t>1e_datum_na_IOW - geconsolideerd</t>
+  </si>
+  <si>
+    <t>1d: datum na_IOW_geconsolideerd  NL.IMRO.0202.EPP976-0301</t>
+  </si>
+  <si>
+    <t>Validatie succesvol</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0000.BZKam11Barro-3025, type = imro:Besluitgebied_A: Fout in typePlan -&gt; Als typePlan is 'amvb' of 'regeling' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'amvb' of 'regeling'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0106.99BHV2020180B-C001, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'beheersverordening' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'beheersverordening'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.1930.BPRaadhuislaanSP-1001, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'bestemmingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld' of 'geconsolideerd', tenzij naam begint met 'TAM-omgevingsplan '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0855.EXP2021001-b001, type = imro:Besluitgebied_X: Fout in planstatus -&gt; Als imro:typePlan is 'exploitatieplan' en datum is groter dan of gelijk aan 2023-01-01, dan mag planstatus niet zijn 'ontwerp', 'concept' of 'voorontwerp'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0000.EZKip18GaswTern-2001, type = imro:Bestemmingsplangebied: Fout in typePlan -&gt; Als typePlan is 'inpassingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'inpassingsplan', tenzij naam begint met 'TAM-projectbesluit '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id , type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'projectbesluit' of 'tijdelijke ontheffing buitenplans' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'projectbesluit' of 'tijdelijke ontheffing buitenplans'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.9923.phVerordening006B-va01, type = imro:Besluitgebied_P: Fout in typePlan -&gt; Als typePlan is 'provinciale verordening' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'provinciale verordening', tenzij naam begint met 'TAM-omgevingsverordening '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.9926.RA0318SLAPPEDEL8A-VA01, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'reactieve aanwijzing' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'reactieve aanwijzing', tenzij naam begint met 'TAM-reactieve interventie '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0000.BZKmr11Rarro-3050, type = imro:Besluitgebied_A: Fout in typePlan -&gt; Als typePlan is 'amvb' of 'regeling' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'amvb' of 'regeling'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0345.UPDeOntmoetingDp7-ow01, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'uitwerkingsplan' of 'wijzigingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld'.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0202.VBB985-0301, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typeplan is voorbereidingsbesluit en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'voorbereidingsbesluit', tenzij naam begint met 'TAM-voorbereidingsbesluit '.</t>
+  </si>
+  <si>
+    <t>IMRO-object met gml:id NL.IMRO.0302.WI01031-ow01, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'uitwerkingsplan' of 'wijzigingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld'.</t>
+  </si>
+  <si>
+    <t>Testresultaat na ontwikkeling</t>
+  </si>
+  <si>
+    <t>1_IOW_toestaan_planstatus_ontwerp</t>
+  </si>
+  <si>
+    <t>1: validatie_IOW_toestaan_planstatus_ontwerp vóór IWT</t>
+  </si>
+  <si>
+    <t>Testbestand niet correct</t>
+  </si>
+  <si>
+    <t>Onterecht doorgelaten</t>
+  </si>
+  <si>
+    <t>(Planobject gml:id = NL.IMRO.0202.EPP976-0301 , type = imro:Besluitgebied_X ) Foutcode RPA15: Attribuut besluitnummer en verwijzingNaarVaststellingsbesluit alleen toegestaan en verplicht vanaf planstatus = vastgesteld of onherroepelijk. (Huidige waarde planstatus: geconsolideerd ) Zie constraint b4, c5, e5, e13, e19 (afhankelijk van het type planobject) van IMRO2012.pdf paragraaf 8.4.</t>
+  </si>
+  <si>
+    <t>Testbestand lijkt in orde</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testresultaat
 interactieve validatie
-pilot.rp.nl</t>
-  </si>
-  <si>
-    <t>1c_datum_na_IOW_ontwerp_TAMuitgebreid</t>
-  </si>
-  <si>
-    <t>1e: datum na_IOW_ontwerp_TAMuitgebreid  NL.IMRO.0000.EZKip18GaswTern-2001</t>
-  </si>
-  <si>
-    <t>1c_datum_na_IOW TAM_uitgebreid</t>
-  </si>
-  <si>
-    <t>1c_datum_na_IOW TAM_uitgebreid - NL.IMRO.9923.phVerordening006B-va01</t>
-  </si>
-  <si>
-    <t>1c_datum_na_IOW_TAM_uitgebreid</t>
-  </si>
-  <si>
-    <t>1c_datum_na_IOW_TAM_uitgebreid - NL.IMRO.9926.RA0318SLAPPEDEL8A-VA01</t>
-  </si>
-  <si>
-    <t>1e_datum_na_IOW - geconsolideerd</t>
-  </si>
-  <si>
-    <t>1d: datum na_IOW_geconsolideerd  NL.IMRO.0202.EPP976-0301</t>
-  </si>
-  <si>
-    <t>Validatie succesvol</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.0000.BZKam11Barro-3025, type = imro:Besluitgebied_A: Fout in typePlan -&gt; Als typePlan is 'amvb' of 'regeling' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'amvb' of 'regeling'.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.0106.99BHV2020180B-C001, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'beheersverordening' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'beheersverordening'.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.1930.BPRaadhuislaanSP-1001, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'bestemmingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld' of 'geconsolideerd', tenzij naam begint met 'TAM-omgevingsplan '.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.0855.EXP2021001-b001, type = imro:Besluitgebied_X: Fout in planstatus -&gt; Als imro:typePlan is 'exploitatieplan' en datum is groter dan of gelijk aan 2023-01-01, dan mag planstatus niet zijn 'ontwerp', 'concept' of 'voorontwerp'.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.0000.EZKip18GaswTern-2001, type = imro:Bestemmingsplangebied: Fout in typePlan -&gt; Als typePlan is 'inpassingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'inpassingsplan', tenzij naam begint met 'TAM-projectbesluit '.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id , type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'projectbesluit' of 'tijdelijke ontheffing buitenplans' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'projectbesluit' of 'tijdelijke ontheffing buitenplans'.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.9923.phVerordening006B-va01, type = imro:Besluitgebied_P: Fout in typePlan -&gt; Als typePlan is 'provinciale verordening' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'provinciale verordening', tenzij naam begint met 'TAM-omgevingsverordening '.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.9926.RA0318SLAPPEDEL8A-VA01, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typePlan is 'reactieve aanwijzing' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'reactieve aanwijzing', tenzij naam begint met 'TAM-reactieve interventie '.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.0000.BZKmr11Rarro-3050, type = imro:Besluitgebied_A: Fout in typePlan -&gt; Als typePlan is 'amvb' of 'regeling' en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'amvb' of 'regeling'.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.0345.UPDeOntmoetingDp7-ow01, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'uitwerkingsplan' of 'wijzigingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld'.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.0202.VBB985-0301, type = imro:Besluitgebied_X: Fout in typePlan -&gt; Als typeplan is voorbereidingsbesluit en datum is groter dan of gelijk aan 2023-01-01, dan mag typePlan niet zijn 'voorbereidingsbesluit', tenzij naam begint met 'TAM-voorbereidingsbesluit '.</t>
-  </si>
-  <si>
-    <t>IMRO-object met gml:id NL.IMRO.0302.WI01031-ow01, type = imro:Bestemmingsplangebied: Fout in planstatus -&gt; Als typePlan is 'uitwerkingsplan' of 'wijzigingsplan' en datum is groter dan of gelijk aan 2023-01-01, dan moet planstatus zijn 'vastgesteld'.</t>
-  </si>
-  <si>
-    <t>Testresultaat na ontwikkeling</t>
-  </si>
-  <si>
-    <t>1_IOW_toestaan_planstatus_ontwerp</t>
-  </si>
-  <si>
-    <t>1: validatie_IOW_toestaan_planstatus_ontwerp vóór IWT</t>
-  </si>
-  <si>
-    <t>Testbestand niet correct</t>
-  </si>
-  <si>
-    <t>Onterecht doorgelaten</t>
-  </si>
-  <si>
-    <t>(Planobject gml:id = NL.IMRO.0202.EPP976-0301 , type = imro:Besluitgebied_X ) Foutcode RPA15: Attribuut besluitnummer en verwijzingNaarVaststellingsbesluit alleen toegestaan en verplicht vanaf planstatus = vastgesteld of onherroepelijk. (Huidige waarde planstatus: geconsolideerd ) Zie constraint b4, c5, e5, e13, e19 (afhankelijk van het type planobject) van IMRO2012.pdf paragraaf 8.4.</t>
-  </si>
-  <si>
-    <t>Testbestand lijkt in orde</t>
-  </si>
-  <si>
-    <t>Testresultaat
+pilot.rp.nl - validatiebestanden opgesplitst in IMRO2008 en 2012
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dd. 12-10-2022</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testresultaat
 interactieve validatie
-pilot.rp.nl - validatiebestanden opgesplitst in IMRO2008 en 2012</t>
+pilot.rp.nl
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dd. 12-10-2022</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -852,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66C8936-D7D1-4C1D-960D-9AD61970D693}">
   <dimension ref="A1:FE53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +895,7 @@
     <col min="9" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:161" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:161" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -881,13 +907,13 @@
         <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>79</v>
@@ -907,13 +933,13 @@
         <v>27</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1082,13 +1108,13 @@
         <v>27</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1259,13 +1285,13 @@
         <v>27</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:161" ht="144" x14ac:dyDescent="0.3">
@@ -1279,13 +1305,13 @@
         <v>28</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:161" x14ac:dyDescent="0.3">
@@ -1302,13 +1328,13 @@
         <v>27</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:161" ht="144" x14ac:dyDescent="0.3">
@@ -1322,13 +1348,13 @@
         <v>28</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:161" x14ac:dyDescent="0.3">
@@ -1336,20 +1362,20 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:161" x14ac:dyDescent="0.3">
@@ -1363,13 +1389,13 @@
         <v>27</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:161" x14ac:dyDescent="0.3">
@@ -1383,13 +1409,13 @@
         <v>27</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:161" ht="187.2" x14ac:dyDescent="0.3">
@@ -1403,13 +1429,13 @@
         <v>39</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:161" ht="187.2" x14ac:dyDescent="0.3">
@@ -1423,13 +1449,13 @@
         <v>39</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:161" ht="187.2" x14ac:dyDescent="0.3">
@@ -1443,13 +1469,13 @@
         <v>39</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:161" x14ac:dyDescent="0.3">
@@ -1463,13 +1489,13 @@
         <v>27</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:161" x14ac:dyDescent="0.3">
@@ -1486,13 +1512,13 @@
         <v>27</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:161" x14ac:dyDescent="0.3">
@@ -1506,13 +1532,13 @@
         <v>27</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:161" ht="158.4" x14ac:dyDescent="0.3">
@@ -1526,13 +1552,13 @@
         <v>28</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:161" x14ac:dyDescent="0.3">
@@ -1546,36 +1572,36 @@
         <v>27</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:161" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="D19" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:161" x14ac:dyDescent="0.3">
@@ -1592,13 +1618,13 @@
         <v>27</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:161" x14ac:dyDescent="0.3">
@@ -1612,13 +1638,13 @@
         <v>27</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:161" x14ac:dyDescent="0.3">
@@ -1635,13 +1661,13 @@
         <v>27</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:161" x14ac:dyDescent="0.3">
@@ -1655,13 +1681,13 @@
         <v>27</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:161" ht="172.8" x14ac:dyDescent="0.3">
@@ -1675,13 +1701,13 @@
         <v>28</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:161" x14ac:dyDescent="0.3">
@@ -1695,33 +1721,33 @@
         <v>27</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:161" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>85</v>
-      </c>
       <c r="D26" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:161" x14ac:dyDescent="0.3">
@@ -1738,13 +1764,13 @@
         <v>27</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:161" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1759,13 +1785,13 @@
         <v>27</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -1936,13 +1962,13 @@
         <v>27</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:161" ht="144" x14ac:dyDescent="0.3">
@@ -1956,16 +1982,16 @@
         <v>28</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:161" x14ac:dyDescent="0.3">
@@ -1982,13 +2008,13 @@
         <v>27</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:161" ht="172.8" x14ac:dyDescent="0.3">
@@ -2002,33 +2028,33 @@
         <v>28</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="D33" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2045,13 +2071,13 @@
         <v>27</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
@@ -2065,33 +2091,33 @@
         <v>28</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="D36" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2108,13 +2134,13 @@
         <v>27</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -2128,13 +2154,13 @@
         <v>28</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2151,13 +2177,13 @@
         <v>27</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2171,13 +2197,13 @@
         <v>27</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2194,13 +2220,13 @@
         <v>27</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -2214,16 +2240,16 @@
         <v>28</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2240,13 +2266,13 @@
         <v>27</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2260,13 +2286,13 @@
         <v>27</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -2280,13 +2306,13 @@
         <v>28</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -2300,13 +2326,13 @@
         <v>27</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -2323,13 +2349,13 @@
         <v>27</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
@@ -2343,13 +2369,13 @@
         <v>39</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H48" s="13"/>
     </row>
@@ -2364,13 +2390,13 @@
         <v>27</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2387,13 +2413,13 @@
         <v>27</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2407,13 +2433,13 @@
         <v>27</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="144" x14ac:dyDescent="0.3">
@@ -2427,13 +2453,13 @@
         <v>28</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2447,13 +2473,13 @@
         <v>27</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2463,15 +2489,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063B796D0CB608148ADB6A3FE6184D975" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="71d6b85c0b6e09903bf280259070e852">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ab01c9f7-308e-412a-8b6b-2a38868f1fe8" xmlns:ns3="f5714f12-861a-48fb-8033-d35a907f947e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f26ee0e1d009816e1c8af2a8a71dce8" ns2:_="" ns3:_="">
     <xsd:import namespace="ab01c9f7-308e-412a-8b6b-2a38868f1fe8"/>
@@ -2660,6 +2677,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2672,14 +2698,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955549FB-6958-4E07-8677-91C492AD0DEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58DE8008-C1B9-4D83-B2C3-04BDD37EF824}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2698,6 +2716,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955549FB-6958-4E07-8677-91C492AD0DEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1DD17D3-045C-46B8-BB98-00D1B5119EE5}">
   <ds:schemaRefs>

</xml_diff>